<commit_message>
mainly about spanning tree method
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -129,7 +129,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
@@ -139,6 +139,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -441,15 +443,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:AK57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:A29"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="AH53" sqref="AH53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2">
         <v>1</v>
@@ -490,8 +492,60 @@
       <c r="N1" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T1" s="1"/>
+      <c r="U1" s="2">
+        <v>1</v>
+      </c>
+      <c r="V1" s="2">
+        <v>2</v>
+      </c>
+      <c r="W1" s="2">
+        <v>3</v>
+      </c>
+      <c r="X1" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y1" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z1" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA1" s="2">
+        <v>7</v>
+      </c>
+      <c r="AB1" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC1" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD1" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE1" s="2">
+        <v>11</v>
+      </c>
+      <c r="AF1" s="2">
+        <v>12</v>
+      </c>
+      <c r="AG1" s="3">
+        <v>13</v>
+      </c>
+      <c r="AH1" s="2">
+        <v>14</v>
+      </c>
+      <c r="AI1" s="3">
+        <v>15</v>
+      </c>
+      <c r="AJ1" s="2">
+        <v>16</v>
+      </c>
+      <c r="AK1" s="9">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -534,8 +588,62 @@
       <c r="N2" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T2" s="4">
+        <v>1</v>
+      </c>
+      <c r="U2" s="5">
+        <v>0</v>
+      </c>
+      <c r="V2" s="5">
+        <v>0</v>
+      </c>
+      <c r="W2" s="5">
+        <v>0</v>
+      </c>
+      <c r="X2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -578,8 +686,62 @@
       <c r="N3" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T3" s="4">
+        <v>2</v>
+      </c>
+      <c r="U3" s="5">
+        <v>0</v>
+      </c>
+      <c r="V3" s="5">
+        <v>0</v>
+      </c>
+      <c r="W3" s="5">
+        <v>0</v>
+      </c>
+      <c r="X3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -622,8 +784,62 @@
       <c r="N4" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T4" s="4">
+        <v>3</v>
+      </c>
+      <c r="U4" s="5">
+        <v>0</v>
+      </c>
+      <c r="V4" s="5">
+        <v>0</v>
+      </c>
+      <c r="W4" s="5">
+        <v>0</v>
+      </c>
+      <c r="X4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -666,8 +882,62 @@
       <c r="N5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T5" s="4">
+        <v>4</v>
+      </c>
+      <c r="U5" s="5">
+        <v>0</v>
+      </c>
+      <c r="V5" s="5">
+        <v>0</v>
+      </c>
+      <c r="W5" s="5">
+        <v>0</v>
+      </c>
+      <c r="X5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -710,8 +980,62 @@
       <c r="N6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T6" s="4">
+        <v>5</v>
+      </c>
+      <c r="U6" s="5">
+        <v>0</v>
+      </c>
+      <c r="V6" s="5">
+        <v>0</v>
+      </c>
+      <c r="W6" s="5">
+        <v>0</v>
+      </c>
+      <c r="X6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -754,8 +1078,62 @@
       <c r="N7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T7" s="4">
+        <v>6</v>
+      </c>
+      <c r="U7" s="5">
+        <v>0</v>
+      </c>
+      <c r="V7" s="5">
+        <v>0</v>
+      </c>
+      <c r="W7" s="5">
+        <v>0</v>
+      </c>
+      <c r="X7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -798,8 +1176,62 @@
       <c r="N8" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T8" s="4">
+        <v>7</v>
+      </c>
+      <c r="U8" s="5">
+        <v>0</v>
+      </c>
+      <c r="V8" s="5">
+        <v>0</v>
+      </c>
+      <c r="W8" s="5">
+        <v>0</v>
+      </c>
+      <c r="X8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -842,8 +1274,62 @@
       <c r="N9" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T9" s="4">
+        <v>8</v>
+      </c>
+      <c r="U9" s="5">
+        <v>0</v>
+      </c>
+      <c r="V9" s="5">
+        <v>0</v>
+      </c>
+      <c r="W9" s="5">
+        <v>0</v>
+      </c>
+      <c r="X9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -886,8 +1372,62 @@
       <c r="N10" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T10" s="4">
+        <v>9</v>
+      </c>
+      <c r="U10" s="5">
+        <v>0</v>
+      </c>
+      <c r="V10" s="5">
+        <v>0</v>
+      </c>
+      <c r="W10" s="5">
+        <v>0</v>
+      </c>
+      <c r="X10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK10" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -930,8 +1470,62 @@
       <c r="N11" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T11" s="4">
+        <v>10</v>
+      </c>
+      <c r="U11" s="5">
+        <v>0</v>
+      </c>
+      <c r="V11" s="5">
+        <v>0</v>
+      </c>
+      <c r="W11" s="5">
+        <v>0</v>
+      </c>
+      <c r="X11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK11" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -974,8 +1568,62 @@
       <c r="N12" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T12" s="4">
+        <v>11</v>
+      </c>
+      <c r="U12" s="5">
+        <v>0</v>
+      </c>
+      <c r="V12" s="5">
+        <v>0</v>
+      </c>
+      <c r="W12" s="5">
+        <v>0</v>
+      </c>
+      <c r="X12" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI12" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ12" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK12" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1018,8 +1666,62 @@
       <c r="N13" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T13" s="4">
+        <v>12</v>
+      </c>
+      <c r="U13" s="5">
+        <v>0</v>
+      </c>
+      <c r="V13" s="5">
+        <v>0</v>
+      </c>
+      <c r="W13" s="5">
+        <v>0</v>
+      </c>
+      <c r="X13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ13" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>13</v>
       </c>
@@ -1062,8 +1764,118 @@
       <c r="N14" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="T14" s="7">
+        <v>13</v>
+      </c>
+      <c r="U14" s="5">
+        <v>0</v>
+      </c>
+      <c r="V14" s="5">
+        <v>0</v>
+      </c>
+      <c r="W14" s="5">
+        <v>0</v>
+      </c>
+      <c r="X14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI14" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ14" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK14" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T15" s="4">
+        <v>14</v>
+      </c>
+      <c r="U15" s="5">
+        <v>0</v>
+      </c>
+      <c r="V15" s="5">
+        <v>0</v>
+      </c>
+      <c r="W15" s="5">
+        <v>0</v>
+      </c>
+      <c r="X15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI15" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="2">
         <v>1</v>
@@ -1083,92 +1895,2182 @@
       <c r="G16" s="2">
         <v>6</v>
       </c>
-      <c r="H16" s="2">
-        <v>7</v>
-      </c>
-      <c r="I16" s="2">
-        <v>8</v>
-      </c>
-      <c r="J16" s="2">
-        <v>9</v>
-      </c>
-      <c r="K16" s="2">
-        <v>10</v>
-      </c>
-      <c r="L16" s="2">
-        <v>11</v>
-      </c>
-      <c r="M16" s="2">
-        <v>12</v>
-      </c>
-      <c r="N16" s="3">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="3"/>
+      <c r="T16" s="4">
+        <v>15</v>
+      </c>
+      <c r="U16" s="5">
+        <v>0</v>
+      </c>
+      <c r="V16" s="5">
+        <v>0</v>
+      </c>
+      <c r="W16" s="5">
+        <v>0</v>
+      </c>
+      <c r="X16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI16" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ16" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="T17" s="7">
+        <v>16</v>
+      </c>
+      <c r="U17" s="5">
+        <v>0</v>
+      </c>
+      <c r="V17" s="5">
+        <v>0</v>
+      </c>
+      <c r="W17" s="5">
+        <v>0</v>
+      </c>
+      <c r="X17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AJ17" s="5">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="T18" s="4">
+        <v>17</v>
+      </c>
+      <c r="U18" s="10">
+        <v>0</v>
+      </c>
+      <c r="V18" s="10">
+        <v>0</v>
+      </c>
+      <c r="W18" s="10">
+        <v>0</v>
+      </c>
+      <c r="X18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AB18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AE18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AF18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AG18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AI18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AJ18" s="10">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="T21" s="1"/>
+      <c r="U21" s="2">
+        <v>1</v>
+      </c>
+      <c r="V21" s="2">
+        <v>2</v>
+      </c>
+      <c r="W21" s="2">
+        <v>3</v>
+      </c>
+      <c r="X21" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y21" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z21" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>7</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC21" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD21" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="3"/>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="T22" s="4">
+        <v>1</v>
+      </c>
+      <c r="U22" s="5">
+        <v>0</v>
+      </c>
+      <c r="V22" s="5">
+        <v>0</v>
+      </c>
+      <c r="W22" s="5">
+        <v>0</v>
+      </c>
+      <c r="X22" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y22" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE22" s="5"/>
+      <c r="AF22" s="5"/>
+      <c r="AG22" s="5"/>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="T23" s="4">
+        <v>2</v>
+      </c>
+      <c r="U23" s="5">
+        <v>0</v>
+      </c>
+      <c r="V23" s="5">
+        <v>0</v>
+      </c>
+      <c r="W23" s="5">
+        <v>0</v>
+      </c>
+      <c r="X23" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y23" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD23" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE23" s="5"/>
+      <c r="AF23" s="5"/>
+      <c r="AG23" s="5"/>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="T24" s="4">
+        <v>3</v>
+      </c>
+      <c r="U24" s="5">
+        <v>0</v>
+      </c>
+      <c r="V24" s="5">
+        <v>0</v>
+      </c>
+      <c r="W24" s="5">
+        <v>0</v>
+      </c>
+      <c r="X24" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="5"/>
+      <c r="AF24" s="5"/>
+      <c r="AG24" s="5"/>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="T25" s="4">
+        <v>4</v>
+      </c>
+      <c r="U25" s="5">
+        <v>0</v>
+      </c>
+      <c r="V25" s="5">
+        <v>0</v>
+      </c>
+      <c r="W25" s="5">
+        <v>0</v>
+      </c>
+      <c r="X25" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y25" s="5">
+        <v>1</v>
+      </c>
+      <c r="Z25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD25" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE25" s="5"/>
+      <c r="AF25" s="5"/>
+      <c r="AG25" s="5"/>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
+      <c r="T26" s="4">
+        <v>5</v>
+      </c>
+      <c r="U26" s="5">
+        <v>0</v>
+      </c>
+      <c r="V26" s="5">
+        <v>0</v>
+      </c>
+      <c r="W26" s="5">
+        <v>0</v>
+      </c>
+      <c r="X26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y26" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC26" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD26" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE26" s="5"/>
+      <c r="AF26" s="5"/>
+      <c r="AG26" s="5"/>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="T27" s="4">
+        <v>6</v>
+      </c>
+      <c r="U27" s="5">
+        <v>0</v>
+      </c>
+      <c r="V27" s="5">
+        <v>0</v>
+      </c>
+      <c r="W27" s="5">
+        <v>0</v>
+      </c>
+      <c r="X27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y27" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD27" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE27" s="5"/>
+      <c r="AF27" s="5"/>
+      <c r="AG27" s="5"/>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A28" s="4"/>
+      <c r="T28" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4">
+      <c r="U28" s="5">
+        <v>0</v>
+      </c>
+      <c r="V28" s="5">
+        <v>0</v>
+      </c>
+      <c r="W28" s="5">
+        <v>0</v>
+      </c>
+      <c r="X28" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="5"/>
+      <c r="AF28" s="5"/>
+      <c r="AG28" s="5"/>
+    </row>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
+      <c r="T29" s="4">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="U29" s="5">
+        <v>0</v>
+      </c>
+      <c r="V29" s="5">
+        <v>0</v>
+      </c>
+      <c r="W29" s="5">
+        <v>0</v>
+      </c>
+      <c r="X29" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y29" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB29" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD29" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="5"/>
+      <c r="AF29" s="5"/>
+      <c r="AG29" s="5"/>
+    </row>
+    <row r="30" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T30" s="4">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="U30" s="5">
+        <v>0</v>
+      </c>
+      <c r="V30" s="5">
+        <v>0</v>
+      </c>
+      <c r="W30" s="5">
+        <v>0</v>
+      </c>
+      <c r="X30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y30" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD30" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE30" s="5"/>
+      <c r="AF30" s="5"/>
+      <c r="AG30" s="5"/>
+    </row>
+    <row r="31" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T31" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="U31" s="5">
+        <v>0</v>
+      </c>
+      <c r="V31" s="5">
+        <v>0</v>
+      </c>
+      <c r="W31" s="5">
+        <v>0</v>
+      </c>
+      <c r="X31" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z31" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB31" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD31" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE31" s="5"/>
+      <c r="AF31" s="5"/>
+      <c r="AG31" s="5"/>
+    </row>
+    <row r="32" spans="1:37" x14ac:dyDescent="0.25">
+      <c r="T32" s="4"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
+      <c r="X32" s="5"/>
+      <c r="Y32" s="5"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="5"/>
+      <c r="AB32" s="5"/>
+      <c r="AC32" s="5"/>
+      <c r="AD32" s="5"/>
+      <c r="AE32" s="5"/>
+      <c r="AF32" s="5"/>
+      <c r="AG32" s="6"/>
+    </row>
+    <row r="33" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T33" s="4"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
+      <c r="X33" s="5"/>
+      <c r="Y33" s="5"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="5"/>
+      <c r="AC33" s="5"/>
+      <c r="AD33" s="5"/>
+      <c r="AE33" s="5"/>
+      <c r="AF33" s="5"/>
+      <c r="AG33" s="6"/>
+    </row>
+    <row r="34" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T34" s="7"/>
+      <c r="U34" s="8"/>
+      <c r="V34" s="8"/>
+      <c r="W34" s="8"/>
+      <c r="X34" s="8"/>
+      <c r="Y34" s="8"/>
+      <c r="Z34" s="8"/>
+      <c r="AA34" s="8"/>
+      <c r="AB34" s="8"/>
+      <c r="AC34" s="8"/>
+      <c r="AD34" s="8"/>
+      <c r="AE34" s="8"/>
+      <c r="AF34" s="8"/>
+      <c r="AG34" s="8"/>
+    </row>
+    <row r="36" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B36" s="1"/>
+      <c r="C36" s="2">
+        <v>1</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+      <c r="E36" s="2">
+        <v>3</v>
+      </c>
+      <c r="F36" s="2">
+        <v>4</v>
+      </c>
+      <c r="G36" s="2">
+        <v>5</v>
+      </c>
+      <c r="H36" s="2">
+        <v>6</v>
+      </c>
+      <c r="I36" s="2">
+        <v>7</v>
+      </c>
+      <c r="J36" s="2">
+        <v>8</v>
+      </c>
+      <c r="K36" s="2">
+        <v>9</v>
+      </c>
+      <c r="L36" s="2">
+        <v>10</v>
+      </c>
+      <c r="M36" s="2">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="N36" s="2">
         <v>12</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
+      <c r="O36" s="3">
         <v>13</v>
       </c>
+    </row>
+    <row r="37" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <v>0</v>
+      </c>
+      <c r="D37" s="5">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>0</v>
+      </c>
+      <c r="F37" s="5">
+        <v>0</v>
+      </c>
+      <c r="G37" s="5">
+        <v>1</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <v>0</v>
+      </c>
+      <c r="K37" s="5">
+        <v>0</v>
+      </c>
+      <c r="L37" s="5">
+        <v>0</v>
+      </c>
+      <c r="M37" s="5">
+        <v>0</v>
+      </c>
+      <c r="N37" s="5">
+        <v>0</v>
+      </c>
+      <c r="O37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B38" s="4">
+        <v>2</v>
+      </c>
+      <c r="C38" s="5">
+        <v>0</v>
+      </c>
+      <c r="D38" s="5">
+        <v>0</v>
+      </c>
+      <c r="E38" s="5">
+        <v>0</v>
+      </c>
+      <c r="F38" s="5">
+        <v>0</v>
+      </c>
+      <c r="G38" s="5">
+        <v>1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
+        <v>0</v>
+      </c>
+      <c r="K38" s="5">
+        <v>0</v>
+      </c>
+      <c r="L38" s="5">
+        <v>0</v>
+      </c>
+      <c r="M38" s="5">
+        <v>0</v>
+      </c>
+      <c r="N38" s="5">
+        <v>0</v>
+      </c>
+      <c r="O38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B39" s="4">
+        <v>3</v>
+      </c>
+      <c r="C39" s="5">
+        <v>0</v>
+      </c>
+      <c r="D39" s="5">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>0</v>
+      </c>
+      <c r="F39" s="5">
+        <v>0</v>
+      </c>
+      <c r="G39" s="5">
+        <v>1</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5">
+        <v>0</v>
+      </c>
+      <c r="K39" s="5">
+        <v>0</v>
+      </c>
+      <c r="L39" s="5">
+        <v>0</v>
+      </c>
+      <c r="M39" s="5">
+        <v>0</v>
+      </c>
+      <c r="N39" s="5">
+        <v>0</v>
+      </c>
+      <c r="O39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B40" s="4">
+        <v>4</v>
+      </c>
+      <c r="C40" s="5">
+        <v>0</v>
+      </c>
+      <c r="D40" s="5">
+        <v>0</v>
+      </c>
+      <c r="E40" s="5">
+        <v>0</v>
+      </c>
+      <c r="F40" s="5">
+        <v>0</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0</v>
+      </c>
+      <c r="H40" s="5">
+        <v>1</v>
+      </c>
+      <c r="I40" s="5">
+        <v>1</v>
+      </c>
+      <c r="J40" s="5">
+        <v>1</v>
+      </c>
+      <c r="K40" s="5">
+        <v>0</v>
+      </c>
+      <c r="L40" s="5">
+        <v>0</v>
+      </c>
+      <c r="M40" s="5">
+        <v>0</v>
+      </c>
+      <c r="N40" s="5">
+        <v>0</v>
+      </c>
+      <c r="O40" s="5">
+        <v>0</v>
+      </c>
+      <c r="T40" s="1"/>
+      <c r="U40" s="2">
+        <v>1</v>
+      </c>
+      <c r="V40" s="2">
+        <v>2</v>
+      </c>
+      <c r="W40" s="2">
+        <v>3</v>
+      </c>
+      <c r="X40" s="2">
+        <v>4</v>
+      </c>
+      <c r="Y40" s="2">
+        <v>5</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>6</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>7</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>8</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>9</v>
+      </c>
+      <c r="AD40" s="2">
+        <v>10</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>11</v>
+      </c>
+      <c r="AF40" s="2">
+        <v>12</v>
+      </c>
+      <c r="AG40" s="3">
+        <v>13</v>
+      </c>
+      <c r="AH40" s="2">
+        <v>14</v>
+      </c>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="2"/>
+      <c r="AK40" s="9"/>
+    </row>
+    <row r="41" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B41" s="4">
+        <v>5</v>
+      </c>
+      <c r="C41" s="5">
+        <v>0</v>
+      </c>
+      <c r="D41" s="5">
+        <v>0</v>
+      </c>
+      <c r="E41" s="5">
+        <v>0</v>
+      </c>
+      <c r="F41" s="5">
+        <v>0</v>
+      </c>
+      <c r="G41" s="5">
+        <v>0</v>
+      </c>
+      <c r="H41" s="5">
+        <v>0</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <v>0</v>
+      </c>
+      <c r="K41" s="5">
+        <v>1</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0</v>
+      </c>
+      <c r="M41" s="5">
+        <v>0</v>
+      </c>
+      <c r="N41" s="5">
+        <v>0</v>
+      </c>
+      <c r="O41" s="5">
+        <v>0</v>
+      </c>
+      <c r="T41" s="4">
+        <v>1</v>
+      </c>
+      <c r="U41" s="5">
+        <v>0</v>
+      </c>
+      <c r="V41" s="5">
+        <v>0</v>
+      </c>
+      <c r="W41" s="5">
+        <v>0</v>
+      </c>
+      <c r="X41" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y41" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH41" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI41" s="5"/>
+      <c r="AJ41" s="5"/>
+      <c r="AK41" s="10"/>
+    </row>
+    <row r="42" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B42" s="4">
+        <v>6</v>
+      </c>
+      <c r="C42" s="5">
+        <v>0</v>
+      </c>
+      <c r="D42" s="5">
+        <v>0</v>
+      </c>
+      <c r="E42" s="5">
+        <v>0</v>
+      </c>
+      <c r="F42" s="5">
+        <v>0</v>
+      </c>
+      <c r="G42" s="5">
+        <v>0</v>
+      </c>
+      <c r="H42" s="5">
+        <v>0</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>0</v>
+      </c>
+      <c r="K42" s="5">
+        <v>0</v>
+      </c>
+      <c r="L42" s="5">
+        <v>1</v>
+      </c>
+      <c r="M42" s="5">
+        <v>0</v>
+      </c>
+      <c r="N42" s="5">
+        <v>0</v>
+      </c>
+      <c r="O42" s="5">
+        <v>0</v>
+      </c>
+      <c r="T42" s="4">
+        <v>2</v>
+      </c>
+      <c r="U42" s="5">
+        <v>0</v>
+      </c>
+      <c r="V42" s="5">
+        <v>0</v>
+      </c>
+      <c r="W42" s="5">
+        <v>0</v>
+      </c>
+      <c r="X42" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y42" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="5">
+        <v>1</v>
+      </c>
+      <c r="AA42" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="5"/>
+      <c r="AJ42" s="5"/>
+      <c r="AK42" s="10"/>
+    </row>
+    <row r="43" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B43" s="4">
+        <v>7</v>
+      </c>
+      <c r="C43" s="5">
+        <v>0</v>
+      </c>
+      <c r="D43" s="5">
+        <v>0</v>
+      </c>
+      <c r="E43" s="5">
+        <v>0</v>
+      </c>
+      <c r="F43" s="5">
+        <v>0</v>
+      </c>
+      <c r="G43" s="5">
+        <v>0</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0</v>
+      </c>
+      <c r="I43" s="5">
+        <v>0</v>
+      </c>
+      <c r="J43" s="5">
+        <v>0</v>
+      </c>
+      <c r="K43" s="5">
+        <v>0</v>
+      </c>
+      <c r="L43" s="5">
+        <v>0</v>
+      </c>
+      <c r="M43" s="5">
+        <v>1</v>
+      </c>
+      <c r="N43" s="5">
+        <v>0</v>
+      </c>
+      <c r="O43" s="5">
+        <v>0</v>
+      </c>
+      <c r="T43" s="4">
+        <v>3</v>
+      </c>
+      <c r="U43" s="5">
+        <v>0</v>
+      </c>
+      <c r="V43" s="5">
+        <v>0</v>
+      </c>
+      <c r="W43" s="5">
+        <v>0</v>
+      </c>
+      <c r="X43" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="5">
+        <v>1</v>
+      </c>
+      <c r="AB43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF43" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH43" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI43" s="5"/>
+      <c r="AJ43" s="5"/>
+      <c r="AK43" s="10"/>
+    </row>
+    <row r="44" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B44" s="4">
+        <v>8</v>
+      </c>
+      <c r="C44" s="5">
+        <v>0</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0</v>
+      </c>
+      <c r="E44" s="5">
+        <v>0</v>
+      </c>
+      <c r="F44" s="5">
+        <v>0</v>
+      </c>
+      <c r="G44" s="5">
+        <v>0</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0</v>
+      </c>
+      <c r="I44" s="5">
+        <v>0</v>
+      </c>
+      <c r="J44" s="5">
+        <v>0</v>
+      </c>
+      <c r="K44" s="5">
+        <v>0</v>
+      </c>
+      <c r="L44" s="5">
+        <v>0</v>
+      </c>
+      <c r="M44" s="5">
+        <v>0</v>
+      </c>
+      <c r="N44" s="5">
+        <v>1</v>
+      </c>
+      <c r="O44" s="5">
+        <v>0</v>
+      </c>
+      <c r="T44" s="4">
+        <v>4</v>
+      </c>
+      <c r="U44" s="5">
+        <v>0</v>
+      </c>
+      <c r="V44" s="5">
+        <v>0</v>
+      </c>
+      <c r="W44" s="5">
+        <v>0</v>
+      </c>
+      <c r="X44" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="5">
+        <v>1</v>
+      </c>
+      <c r="AC44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH44" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI44" s="5"/>
+      <c r="AJ44" s="5"/>
+      <c r="AK44" s="10"/>
+    </row>
+    <row r="45" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B45" s="4">
+        <v>9</v>
+      </c>
+      <c r="C45" s="5">
+        <v>0</v>
+      </c>
+      <c r="D45" s="5">
+        <v>0</v>
+      </c>
+      <c r="E45" s="5">
+        <v>0</v>
+      </c>
+      <c r="F45" s="5">
+        <v>0</v>
+      </c>
+      <c r="G45" s="5">
+        <v>0</v>
+      </c>
+      <c r="H45" s="5">
+        <v>0</v>
+      </c>
+      <c r="I45" s="5">
+        <v>0</v>
+      </c>
+      <c r="J45" s="5">
+        <v>0</v>
+      </c>
+      <c r="K45" s="5">
+        <v>0</v>
+      </c>
+      <c r="L45" s="5">
+        <v>0</v>
+      </c>
+      <c r="M45" s="5">
+        <v>0</v>
+      </c>
+      <c r="N45" s="5">
+        <v>0</v>
+      </c>
+      <c r="O45" s="5">
+        <v>1</v>
+      </c>
+      <c r="T45" s="4">
+        <v>5</v>
+      </c>
+      <c r="U45" s="5">
+        <v>0</v>
+      </c>
+      <c r="V45" s="5">
+        <v>0</v>
+      </c>
+      <c r="W45" s="5">
+        <v>0</v>
+      </c>
+      <c r="X45" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="5">
+        <v>1</v>
+      </c>
+      <c r="AD45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE45" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH45" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI45" s="5"/>
+      <c r="AJ45" s="5"/>
+      <c r="AK45" s="10"/>
+    </row>
+    <row r="46" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B46" s="4">
+        <v>10</v>
+      </c>
+      <c r="C46" s="5">
+        <v>0</v>
+      </c>
+      <c r="D46" s="5">
+        <v>0</v>
+      </c>
+      <c r="E46" s="5">
+        <v>0</v>
+      </c>
+      <c r="F46" s="5">
+        <v>0</v>
+      </c>
+      <c r="G46" s="5">
+        <v>0</v>
+      </c>
+      <c r="H46" s="5">
+        <v>0</v>
+      </c>
+      <c r="I46" s="5">
+        <v>0</v>
+      </c>
+      <c r="J46" s="5">
+        <v>0</v>
+      </c>
+      <c r="K46" s="5">
+        <v>0</v>
+      </c>
+      <c r="L46" s="5">
+        <v>0</v>
+      </c>
+      <c r="M46" s="5">
+        <v>0</v>
+      </c>
+      <c r="N46" s="5">
+        <v>0</v>
+      </c>
+      <c r="O46" s="5">
+        <v>1</v>
+      </c>
+      <c r="T46" s="4">
+        <v>6</v>
+      </c>
+      <c r="U46" s="5">
+        <v>0</v>
+      </c>
+      <c r="V46" s="5">
+        <v>0</v>
+      </c>
+      <c r="W46" s="5">
+        <v>0</v>
+      </c>
+      <c r="X46" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="5">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH46" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI46" s="5"/>
+      <c r="AJ46" s="5"/>
+      <c r="AK46" s="10"/>
+    </row>
+    <row r="47" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B47" s="4">
+        <v>11</v>
+      </c>
+      <c r="C47" s="5">
+        <v>0</v>
+      </c>
+      <c r="D47" s="5">
+        <v>0</v>
+      </c>
+      <c r="E47" s="5">
+        <v>0</v>
+      </c>
+      <c r="F47" s="5">
+        <v>0</v>
+      </c>
+      <c r="G47" s="5">
+        <v>0</v>
+      </c>
+      <c r="H47" s="5">
+        <v>0</v>
+      </c>
+      <c r="I47" s="5">
+        <v>0</v>
+      </c>
+      <c r="J47" s="5">
+        <v>0</v>
+      </c>
+      <c r="K47" s="5">
+        <v>0</v>
+      </c>
+      <c r="L47" s="5">
+        <v>0</v>
+      </c>
+      <c r="M47" s="5">
+        <v>0</v>
+      </c>
+      <c r="N47" s="5">
+        <v>0</v>
+      </c>
+      <c r="O47" s="5">
+        <v>1</v>
+      </c>
+      <c r="T47" s="4">
+        <v>7</v>
+      </c>
+      <c r="U47" s="5">
+        <v>0</v>
+      </c>
+      <c r="V47" s="5">
+        <v>0</v>
+      </c>
+      <c r="W47" s="5">
+        <v>0</v>
+      </c>
+      <c r="X47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE47" s="5">
+        <v>1</v>
+      </c>
+      <c r="AF47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH47" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="10"/>
+    </row>
+    <row r="48" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B48" s="4">
+        <v>12</v>
+      </c>
+      <c r="C48" s="5">
+        <v>0</v>
+      </c>
+      <c r="D48" s="5">
+        <v>0</v>
+      </c>
+      <c r="E48" s="5">
+        <v>0</v>
+      </c>
+      <c r="F48" s="5">
+        <v>0</v>
+      </c>
+      <c r="G48" s="5">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <v>0</v>
+      </c>
+      <c r="I48" s="5">
+        <v>0</v>
+      </c>
+      <c r="J48" s="5">
+        <v>0</v>
+      </c>
+      <c r="K48" s="5">
+        <v>0</v>
+      </c>
+      <c r="L48" s="5">
+        <v>0</v>
+      </c>
+      <c r="M48" s="5">
+        <v>0</v>
+      </c>
+      <c r="N48" s="5">
+        <v>0</v>
+      </c>
+      <c r="O48" s="5">
+        <v>1</v>
+      </c>
+      <c r="T48" s="4">
+        <v>8</v>
+      </c>
+      <c r="U48" s="5">
+        <v>0</v>
+      </c>
+      <c r="V48" s="5">
+        <v>0</v>
+      </c>
+      <c r="W48" s="5">
+        <v>0</v>
+      </c>
+      <c r="X48" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF48" s="5">
+        <v>1</v>
+      </c>
+      <c r="AG48" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH48" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="10"/>
+    </row>
+    <row r="49" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="B49" s="7">
+        <v>13</v>
+      </c>
+      <c r="C49" s="5">
+        <v>0</v>
+      </c>
+      <c r="D49" s="5">
+        <v>0</v>
+      </c>
+      <c r="E49" s="5">
+        <v>0</v>
+      </c>
+      <c r="F49" s="5">
+        <v>0</v>
+      </c>
+      <c r="G49" s="5">
+        <v>0</v>
+      </c>
+      <c r="H49" s="5">
+        <v>0</v>
+      </c>
+      <c r="I49" s="5">
+        <v>0</v>
+      </c>
+      <c r="J49" s="5">
+        <v>0</v>
+      </c>
+      <c r="K49" s="5">
+        <v>0</v>
+      </c>
+      <c r="L49" s="5">
+        <v>0</v>
+      </c>
+      <c r="M49" s="5">
+        <v>0</v>
+      </c>
+      <c r="N49" s="5">
+        <v>0</v>
+      </c>
+      <c r="O49" s="5">
+        <v>0</v>
+      </c>
+      <c r="T49" s="4">
+        <v>9</v>
+      </c>
+      <c r="U49" s="5">
+        <v>0</v>
+      </c>
+      <c r="V49" s="5">
+        <v>0</v>
+      </c>
+      <c r="W49" s="5">
+        <v>0</v>
+      </c>
+      <c r="X49" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y49" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG49" s="5">
+        <v>1</v>
+      </c>
+      <c r="AH49" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI49" s="5"/>
+      <c r="AJ49" s="5"/>
+      <c r="AK49" s="10"/>
+    </row>
+    <row r="50" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T50" s="4">
+        <v>10</v>
+      </c>
+      <c r="U50" s="5">
+        <v>0</v>
+      </c>
+      <c r="V50" s="5">
+        <v>0</v>
+      </c>
+      <c r="W50" s="5">
+        <v>0</v>
+      </c>
+      <c r="X50" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y50" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG50" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH50" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI50" s="5"/>
+      <c r="AJ50" s="10"/>
+      <c r="AK50" s="5"/>
+    </row>
+    <row r="51" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T51" s="4">
+        <v>11</v>
+      </c>
+      <c r="U51" s="5">
+        <v>0</v>
+      </c>
+      <c r="V51" s="5">
+        <v>0</v>
+      </c>
+      <c r="W51" s="5">
+        <v>0</v>
+      </c>
+      <c r="X51" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y51" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG51" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH51" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI51" s="5"/>
+      <c r="AJ51" s="10"/>
+      <c r="AK51" s="5"/>
+    </row>
+    <row r="52" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T52" s="4">
+        <v>12</v>
+      </c>
+      <c r="U52" s="5">
+        <v>0</v>
+      </c>
+      <c r="V52" s="5">
+        <v>0</v>
+      </c>
+      <c r="W52" s="5">
+        <v>0</v>
+      </c>
+      <c r="X52" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y52" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG52" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH52" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI52" s="5"/>
+      <c r="AJ52" s="10"/>
+      <c r="AK52" s="5"/>
+    </row>
+    <row r="53" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T53" s="7">
+        <v>13</v>
+      </c>
+      <c r="U53" s="5">
+        <v>0</v>
+      </c>
+      <c r="V53" s="5">
+        <v>0</v>
+      </c>
+      <c r="W53" s="5">
+        <v>0</v>
+      </c>
+      <c r="X53" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y53" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG53" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH53" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI53" s="5"/>
+      <c r="AJ53" s="10"/>
+      <c r="AK53" s="5"/>
+    </row>
+    <row r="54" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T54" s="4">
+        <v>14</v>
+      </c>
+      <c r="U54" s="5">
+        <v>0</v>
+      </c>
+      <c r="V54" s="5">
+        <v>0</v>
+      </c>
+      <c r="W54" s="5">
+        <v>0</v>
+      </c>
+      <c r="X54" s="5">
+        <v>0</v>
+      </c>
+      <c r="Y54" s="5">
+        <v>0</v>
+      </c>
+      <c r="Z54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AA54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AB54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AD54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AE54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AF54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AG54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AH54" s="5">
+        <v>0</v>
+      </c>
+      <c r="AI54" s="5"/>
+      <c r="AJ54" s="10"/>
+      <c r="AK54" s="5"/>
+    </row>
+    <row r="55" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T55" s="4"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+      <c r="W55" s="5"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="5"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="5"/>
+      <c r="AE55" s="5"/>
+      <c r="AF55" s="5"/>
+      <c r="AG55" s="5"/>
+      <c r="AH55" s="5"/>
+      <c r="AI55" s="5"/>
+      <c r="AJ55" s="10"/>
+      <c r="AK55" s="5"/>
+    </row>
+    <row r="56" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T56" s="7"/>
+      <c r="U56" s="5"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="5"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="5"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="5"/>
+      <c r="AE56" s="5"/>
+      <c r="AF56" s="5"/>
+      <c r="AG56" s="5"/>
+      <c r="AH56" s="5"/>
+      <c r="AI56" s="5"/>
+      <c r="AJ56" s="5"/>
+      <c r="AK56" s="10"/>
+    </row>
+    <row r="57" spans="2:37" x14ac:dyDescent="0.25">
+      <c r="T57" s="4"/>
+      <c r="U57" s="10"/>
+      <c r="V57" s="10"/>
+      <c r="W57" s="10"/>
+      <c r="X57" s="10"/>
+      <c r="Y57" s="10"/>
+      <c r="Z57" s="10"/>
+      <c r="AA57" s="10"/>
+      <c r="AB57" s="10"/>
+      <c r="AC57" s="10"/>
+      <c r="AD57" s="10"/>
+      <c r="AE57" s="10"/>
+      <c r="AF57" s="10"/>
+      <c r="AG57" s="10"/>
+      <c r="AH57" s="10"/>
+      <c r="AI57" s="10"/>
+      <c r="AJ57" s="10"/>
+      <c r="AK57" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>